<commit_message>
Replaced with US version 2.1 before dropping in WRI's draft Brazil files
</commit_message>
<xml_diff>
--- a/InputData/acronym-key.xlsx
+++ b/InputData/acronym-key.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipP\InputData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18180" windowHeight="8730" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18180" windowHeight="8730"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="3" r:id="rId1"/>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="547">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="566">
   <si>
     <t>Top Level Folder</t>
   </si>
@@ -1130,9 +1125,6 @@
     <t>no need to collect input data for variables to be set via calibration.</t>
   </si>
   <si>
-    <t>Potential Perc Reduction in Proc Emis from Cement, Mass CO2e Avoidable by Marginal Cost</t>
-  </si>
-  <si>
     <t>BIEfIE</t>
   </si>
   <si>
@@ -1589,9 +1581,6 @@
     <t>BNVFE, AVLo, PTFURfE, AVL</t>
   </si>
   <si>
-    <t>high, but included data source supports multiple countries</t>
-  </si>
-  <si>
     <t>BFPIaE</t>
   </si>
   <si>
@@ -1662,12 +1651,75 @@
   </si>
   <si>
     <t>Fraction of Nonenergy Expenditures that Vary with Production</t>
+  </si>
+  <si>
+    <t>EoPPFTSwFP</t>
+  </si>
+  <si>
+    <t>Elasticity of Power Plant Fuel Type Shifting wrt Fuel Price</t>
+  </si>
+  <si>
+    <t>You are modeling a region where power plants can switch the type of fuel they burn in response to fuel price changes without significant plant modifications, such as switching between burning crude oil, heavy fuel oil, and diesel.</t>
+  </si>
+  <si>
+    <t>FSCaFoCC</t>
+  </si>
+  <si>
+    <t>Fuel Shifting Cost as Fraction of Construction Cost</t>
+  </si>
+  <si>
+    <t>Process Emissions Reductions and Costs, Marginal Cost Definitions</t>
+  </si>
+  <si>
+    <t>only adjust country selector (and non-country multipliers, if applicable)</t>
+  </si>
+  <si>
+    <t>BGDP</t>
+  </si>
+  <si>
+    <t>BAU Gross Domestic Product</t>
+  </si>
+  <si>
+    <t>You plan on displaying or using (in Vensim) the emissions-per-unit-GDP or energy-use-per-unit-GDP graphs</t>
+  </si>
+  <si>
+    <t>BTU per Large Primary Energy Unit, BTU per Small Primary Energy Unit</t>
+  </si>
+  <si>
+    <t>geoeng</t>
+  </si>
+  <si>
+    <t>Geoengineering</t>
+  </si>
+  <si>
+    <t>DACD</t>
+  </si>
+  <si>
+    <t>Direct Air Capture Data</t>
+  </si>
+  <si>
+    <t>Direct Air Capture Potential, Direct Air Capture Energy Intensity, Direct Air Capture Amortized CapEx and OM</t>
+  </si>
+  <si>
+    <t>cumulators</t>
+  </si>
+  <si>
+    <t>Cumulators</t>
+  </si>
+  <si>
+    <t>PQS</t>
+  </si>
+  <si>
+    <t>Pollutant Quantization Size</t>
+  </si>
+  <si>
+    <t>Rounding error is visible in final web app output graphs in near-zero pollutant amounts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1735,7 +1787,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1752,11 +1804,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1834,6 +1897,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1899,7 +1977,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1934,7 +2012,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2145,7 +2223,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2237,22 +2315,22 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -2477,11 +2555,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G189"/>
+  <dimension ref="A1:G194"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A116" sqref="A116"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2510,27 +2588,30 @@
         <v>3</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F1" s="27" t="s">
         <v>139</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="33" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>141</v>
+      <c r="B2" s="33" t="s">
+        <v>552</v>
+      </c>
+      <c r="C2" s="33" t="s">
+        <v>553</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>554</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2538,78 +2619,75 @@
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>209</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F4" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B5" s="19" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C5" s="19" t="s">
         <v>210</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20" t="s">
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="G4" s="19"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>140</v>
-      </c>
+      <c r="G5" s="19"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>211</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>212</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>140</v>
+        <v>27</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2617,44 +2695,47 @@
         <v>11</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="F9" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="13" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B10" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>525</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>526</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>527</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>528</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>142</v>
@@ -2665,13 +2746,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>218</v>
+        <v>15</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>141</v>
+        <v>29</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2679,13 +2760,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>142</v>
+        <v>219</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2693,13 +2774,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>16</v>
+        <v>216</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>141</v>
+        <v>217</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2707,86 +2788,83 @@
         <v>11</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>214</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>20</v>
+        <v>214</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>34</v>
+        <v>215</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>436</v>
+        <v>34</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2794,13 +2872,16 @@
         <v>11</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>141</v>
+        <v>35</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2808,16 +2889,13 @@
         <v>11</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>437</v>
+        <v>36</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2825,13 +2903,16 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>141</v>
+        <v>37</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -2839,223 +2920,228 @@
         <v>11</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="F25" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="F24" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+    </row>
+    <row r="26" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B26" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C26" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="21" t="s">
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="21" t="s">
         <v>361</v>
       </c>
-      <c r="G25" s="19"/>
-    </row>
-    <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>141</v>
-      </c>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="F28" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B29" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="C28" s="19" t="s">
+      <c r="C29" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D28" s="19" t="s">
+      <c r="D29" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="19"/>
-      <c r="F28" s="22" t="s">
+      <c r="E29" s="19"/>
+      <c r="F29" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="G28" s="19"/>
-    </row>
-    <row r="29" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="G29" s="19"/>
+    </row>
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B30" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19" t="s">
+      <c r="G30" s="2" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="19" t="s">
         <v>235</v>
       </c>
-      <c r="B30" s="19" t="s">
+      <c r="B31" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C30" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="23" t="s">
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="23" t="s">
         <v>141</v>
       </c>
-      <c r="G30" s="19"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="G31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="34" t="s">
+        <v>561</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>563</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>564</v>
+      </c>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="35" t="s">
+        <v>183</v>
+      </c>
+      <c r="G32" s="34" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C33" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F33" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B34" s="2" t="s">
         <v>281</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F34" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="33" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+    <row r="35" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B35" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C35" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="29" t="s">
+      <c r="F35" s="29" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="34" spans="1:7" s="30" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="25" t="s">
+    <row r="36" spans="1:7" s="30" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B34" s="25" t="s">
+      <c r="B36" s="25" t="s">
+        <v>528</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>529</v>
+      </c>
+      <c r="D36" s="25"/>
+      <c r="E36" s="25"/>
+      <c r="F36" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="G36" s="25" t="s">
         <v>530</v>
-      </c>
-      <c r="C34" s="25" t="s">
-        <v>531</v>
-      </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="24" t="s">
-        <v>421</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>532</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>204</v>
-      </c>
-      <c r="F35" s="16" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="F36" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3063,30 +3149,27 @@
         <v>55</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>451</v>
+        <v>203</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>204</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F38" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>440</v>
+        <v>246</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3094,27 +3177,30 @@
         <v>55</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>261</v>
+        <v>450</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="F39" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>258</v>
+        <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>142</v>
+        <v>70</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3122,13 +3208,13 @@
         <v>55</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>382</v>
+        <v>261</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>140</v>
+        <v>262</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3136,30 +3222,27 @@
         <v>55</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>57</v>
+        <v>258</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>238</v>
+        <v>381</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="F43" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G43" s="2" t="s">
-        <v>440</v>
+        <v>382</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3167,30 +3250,30 @@
         <v>55</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>231</v>
+        <v>57</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>306</v>
+        <v>238</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>305</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>140</v>
+        <v>237</v>
+      </c>
+      <c r="F45" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3198,30 +3281,30 @@
         <v>55</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>58</v>
+        <v>231</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F46" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>59</v>
+        <v>306</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F47" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G47" s="13" t="s">
-        <v>443</v>
+        <v>305</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3229,27 +3312,30 @@
         <v>55</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>266</v>
+        <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>267</v>
+        <v>72</v>
       </c>
       <c r="F48" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>201</v>
+        <v>59</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="F49" s="4" t="s">
-        <v>140</v>
+        <v>73</v>
+      </c>
+      <c r="F49" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3257,30 +3343,27 @@
         <v>55</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>60</v>
+        <v>266</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>74</v>
+        <v>267</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>61</v>
+        <v>201</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>142</v>
+        <v>202</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3288,128 +3371,131 @@
         <v>55</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>429</v>
+        <v>60</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>63</v>
+        <v>428</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>429</v>
+      </c>
+      <c r="F54" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>401</v>
+        <v>62</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>224</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" s="3"/>
       <c r="F56" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>64</v>
+        <v>400</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>374</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="F58" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+        <v>222</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>412</v>
-      </c>
-      <c r="F59" s="5" t="s">
-        <v>265</v>
+        <v>545</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="F59" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>547</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3417,44 +3503,44 @@
         <v>55</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>415</v>
+        <v>64</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>240</v>
+        <v>373</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F61" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>205</v>
+        <v>65</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F62" s="14" t="s">
-        <v>353</v>
+        <v>79</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3462,13 +3548,13 @@
         <v>55</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>66</v>
+        <v>414</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F63" s="4" t="s">
-        <v>140</v>
+        <v>415</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3476,27 +3562,30 @@
         <v>55</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>276</v>
+        <v>548</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>288</v>
+        <v>549</v>
       </c>
       <c r="F64" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>67</v>
+        <v>240</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>142</v>
+        <v>239</v>
+      </c>
+      <c r="F65" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3504,13 +3593,13 @@
         <v>55</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>141</v>
+        <v>206</v>
+      </c>
+      <c r="F66" s="14" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3518,30 +3607,27 @@
         <v>55</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>207</v>
+        <v>66</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F67" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>68</v>
+        <v>276</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F68" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>444</v>
+        <v>288</v>
+      </c>
+      <c r="F68" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3549,13 +3635,13 @@
         <v>55</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>256</v>
+        <v>67</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="F69" s="4" t="s">
-        <v>140</v>
+        <v>81</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3563,75 +3649,72 @@
         <v>55</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>252</v>
+        <v>233</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>253</v>
+        <v>234</v>
       </c>
       <c r="F70" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>283</v>
+        <v>207</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+        <v>208</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>254</v>
+        <v>68</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+      <c r="F72" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="F73" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>257</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>55</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>220</v>
+        <v>252</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="F74" s="4" t="s">
-        <v>140</v>
+        <v>253</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3639,101 +3722,107 @@
         <v>55</v>
       </c>
       <c r="B75" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F76" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="F77" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C75" s="2" t="s">
+      <c r="C79" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F75" s="6" t="s">
+      <c r="F79" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="19" t="s">
+    <row r="80" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="19" t="s">
+      <c r="B80" s="19" t="s">
+        <v>481</v>
+      </c>
+      <c r="C80" s="19" t="s">
         <v>482</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="D80" s="19" t="s">
         <v>483</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="E80" s="19"/>
+      <c r="F80" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="G80" s="19" t="s">
         <v>484</v>
-      </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="24" t="s">
-        <v>421</v>
-      </c>
-      <c r="G76" s="19" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B77" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="F77" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B78" s="2" t="s">
-        <v>376</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>377</v>
-      </c>
-      <c r="F78" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B79" s="2" t="s">
-        <v>380</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>381</v>
-      </c>
-      <c r="F79" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="2" t="s">
-        <v>384</v>
-      </c>
-      <c r="B80" s="2" t="s">
-        <v>378</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>379</v>
-      </c>
-      <c r="F80" s="5" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="F81" s="5" t="s">
         <v>141</v>
@@ -3741,140 +3830,131 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>249</v>
+        <v>375</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>248</v>
+        <v>376</v>
       </c>
       <c r="F82" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>250</v>
+        <v>379</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>251</v>
+        <v>380</v>
       </c>
       <c r="F83" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>268</v>
+        <v>377</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>269</v>
+        <v>378</v>
       </c>
       <c r="F84" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="19" t="s">
-        <v>384</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>404</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>405</v>
-      </c>
-      <c r="D85" s="19"/>
-      <c r="E85" s="19"/>
-      <c r="F85" s="23" t="s">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="F85" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>84</v>
+        <v>383</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>85</v>
+        <v>249</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="F86" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+      <c r="F86" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>84</v>
+        <v>383</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>523</v>
+        <v>250</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="F87" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>84</v>
+        <v>383</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>86</v>
+        <v>268</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>372</v>
-      </c>
-      <c r="F88" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A89" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>310</v>
-      </c>
-      <c r="F89" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>269</v>
+      </c>
+      <c r="F88" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="19" t="s">
+        <v>383</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>403</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>404</v>
+      </c>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G89" s="19"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>491</v>
+        <v>85</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="F90" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="G90" s="2" t="s">
-        <v>493</v>
+        <v>89</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -3882,30 +3962,33 @@
         <v>84</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>433</v>
+        <v>521</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>434</v>
-      </c>
-      <c r="F91" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>522</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F92" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="G92" s="2" t="s">
-        <v>462</v>
+        <v>90</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,13 +3996,13 @@
         <v>84</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>431</v>
+        <v>309</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>432</v>
-      </c>
-      <c r="F93" s="6" t="s">
-        <v>142</v>
+        <v>310</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3927,33 +4010,30 @@
         <v>84</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>536</v>
+        <v>490</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="F94" s="18" t="s">
-        <v>421</v>
+        <v>491</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="G94" s="2" t="s">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>537</v>
+        <v>432</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>540</v>
-      </c>
-      <c r="F95" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G95" s="2" t="s">
-        <v>543</v>
+        <v>433</v>
+      </c>
+      <c r="F95" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -3961,271 +4041,276 @@
         <v>84</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>538</v>
+        <v>87</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>541</v>
-      </c>
-      <c r="F96" s="18" t="s">
-        <v>421</v>
+        <v>91</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>183</v>
       </c>
       <c r="G96" s="2" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>84</v>
       </c>
       <c r="B97" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>431</v>
+      </c>
+      <c r="F97" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A98" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="F98" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G98" s="2" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>535</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>538</v>
+      </c>
+      <c r="F99" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G99" s="2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="F100" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G100" s="2" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A101" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="C101" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D97" s="2" t="s">
+      <c r="D101" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F97" s="4" t="s">
+      <c r="F101" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A98" s="28" t="s">
+    <row r="102" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A102" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="B98" s="28" t="s">
-        <v>516</v>
-      </c>
-      <c r="C98" s="28" t="s">
+      <c r="B102" s="28" t="s">
+        <v>515</v>
+      </c>
+      <c r="C102" s="28" t="s">
+        <v>464</v>
+      </c>
+      <c r="D102" s="28" t="s">
         <v>465</v>
       </c>
-      <c r="D98" s="28" t="s">
-        <v>466</v>
-      </c>
-      <c r="E98" s="28"/>
-      <c r="F98" s="29" t="s">
+      <c r="E102" s="28"/>
+      <c r="F102" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="G98" s="28"/>
-    </row>
-    <row r="99" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="19" t="s">
+      <c r="G102" s="28"/>
+    </row>
+    <row r="103" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B99" s="19" t="s">
-        <v>534</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>535</v>
-      </c>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
-      <c r="F99" s="22" t="s">
+      <c r="B103" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="C103" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="D103" s="19"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="G99" s="19"/>
-    </row>
-    <row r="100" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="B100" s="13" t="s">
-        <v>499</v>
-      </c>
-      <c r="C100" s="13" t="s">
-        <v>506</v>
-      </c>
-      <c r="F100" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="B101" s="13" t="s">
-        <v>500</v>
-      </c>
-      <c r="C101" s="13" t="s">
-        <v>507</v>
-      </c>
-      <c r="F101" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="102" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="B102" s="13" t="s">
-        <v>501</v>
-      </c>
-      <c r="C102" s="13" t="s">
-        <v>508</v>
-      </c>
-      <c r="F102" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="B103" s="13" t="s">
-        <v>502</v>
-      </c>
-      <c r="C103" s="13" t="s">
-        <v>509</v>
-      </c>
-      <c r="D103" s="13" t="s">
-        <v>513</v>
-      </c>
-      <c r="F103" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A104" s="13" t="s">
-        <v>497</v>
-      </c>
-      <c r="B104" s="13" t="s">
-        <v>503</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>510</v>
-      </c>
-      <c r="F104" s="5" t="s">
-        <v>141</v>
-      </c>
+      <c r="G103" s="19"/>
+    </row>
+    <row r="104" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="34" t="s">
+        <v>556</v>
+      </c>
+      <c r="B104" s="34" t="s">
+        <v>558</v>
+      </c>
+      <c r="C104" s="34" t="s">
+        <v>559</v>
+      </c>
+      <c r="D104" s="34" t="s">
+        <v>560</v>
+      </c>
+      <c r="E104" s="34"/>
+      <c r="F104" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G104" s="34"/>
     </row>
     <row r="105" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B105" s="13" t="s">
+        <v>498</v>
+      </c>
+      <c r="C105" s="13" t="s">
+        <v>505</v>
+      </c>
+      <c r="F105" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A106" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="B106" s="13" t="s">
+        <v>499</v>
+      </c>
+      <c r="C106" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="F106" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="B107" s="13" t="s">
+        <v>500</v>
+      </c>
+      <c r="C107" s="13" t="s">
+        <v>507</v>
+      </c>
+      <c r="F107" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="B108" s="13" t="s">
+        <v>501</v>
+      </c>
+      <c r="C108" s="13" t="s">
+        <v>508</v>
+      </c>
+      <c r="D108" s="13" t="s">
+        <v>512</v>
+      </c>
+      <c r="F108" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="B109" s="13" t="s">
+        <v>502</v>
+      </c>
+      <c r="C109" s="13" t="s">
+        <v>509</v>
+      </c>
+      <c r="F109" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="13" t="s">
+        <v>496</v>
+      </c>
+      <c r="B110" s="13" t="s">
+        <v>503</v>
+      </c>
+      <c r="C110" s="13" t="s">
+        <v>510</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G110" s="13" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="25" t="s">
+        <v>496</v>
+      </c>
+      <c r="B111" s="25" t="s">
         <v>504</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="C111" s="25" t="s">
         <v>511</v>
       </c>
-      <c r="F105" s="7" t="s">
+      <c r="D111" s="25"/>
+      <c r="E111" s="25"/>
+      <c r="F111" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="G105" s="13" t="s">
+      <c r="G111" s="25" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="106" spans="1:7" s="13" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="25" t="s">
-        <v>497</v>
-      </c>
-      <c r="B106" s="25" t="s">
-        <v>505</v>
-      </c>
-      <c r="C106" s="25" t="s">
-        <v>512</v>
-      </c>
-      <c r="D106" s="25"/>
-      <c r="E106" s="25"/>
-      <c r="F106" s="26" t="s">
-        <v>183</v>
-      </c>
-      <c r="G106" s="25" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="F107" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="D108" s="2" t="s">
-        <v>529</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F108" s="14" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A109" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="C109" s="2" t="s">
-        <v>278</v>
-      </c>
-      <c r="F109" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G109" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A110" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>449</v>
-      </c>
-      <c r="C110" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="F110" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A111" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C111" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="112" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>96</v>
+        <v>286</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>141</v>
+        <v>287</v>
+      </c>
+      <c r="F112" s="14" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="113" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4233,33 +4318,33 @@
         <v>94</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="F113" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+        <v>527</v>
+      </c>
+      <c r="F113" s="31" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>98</v>
+        <v>277</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F114" s="18" t="s">
-        <v>421</v>
+        <v>278</v>
+      </c>
+      <c r="F114" s="32" t="s">
+        <v>420</v>
       </c>
       <c r="G114" s="2" t="s">
-        <v>480</v>
+        <v>463</v>
       </c>
     </row>
     <row r="115" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4267,44 +4352,38 @@
         <v>94</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>488</v>
+        <v>448</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="D115" s="13" t="s">
-        <v>490</v>
-      </c>
-      <c r="E115" s="13"/>
-      <c r="F115" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="116" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>449</v>
+      </c>
+      <c r="F115" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>545</v>
+        <v>227</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="D116" s="13"/>
-      <c r="E116" s="13"/>
+        <v>228</v>
+      </c>
       <c r="F116" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>279</v>
+        <v>96</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>280</v>
+        <v>103</v>
       </c>
       <c r="F117" s="5" t="s">
         <v>141</v>
@@ -4315,33 +4394,33 @@
         <v>94</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="E118" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F118" s="4" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="119" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>372</v>
+      </c>
+      <c r="F118" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>270</v>
+        <v>98</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="F119" s="5" t="s">
-        <v>141</v>
+        <v>105</v>
+      </c>
+      <c r="F119" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G119" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="120" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4349,13 +4428,17 @@
         <v>94</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>390</v>
+        <v>487</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="F120" s="6" t="s">
-        <v>142</v>
+        <v>488</v>
+      </c>
+      <c r="D120" s="13" t="s">
+        <v>489</v>
+      </c>
+      <c r="E120" s="13"/>
+      <c r="F120" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="121" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4363,44 +4446,46 @@
         <v>94</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>391</v>
+        <v>543</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>394</v>
-      </c>
+        <v>544</v>
+      </c>
+      <c r="D121" s="13"/>
+      <c r="E121" s="13"/>
       <c r="F121" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="122" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>392</v>
+        <v>279</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>395</v>
+        <v>280</v>
       </c>
       <c r="F122" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="F123" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G123" s="2" t="s">
-        <v>533</v>
+        <v>106</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="F123" s="31" t="s">
+        <v>551</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4408,134 +4493,131 @@
         <v>94</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>447</v>
+        <v>270</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>448</v>
+        <v>271</v>
       </c>
       <c r="F124" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>94</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>427</v>
+        <v>389</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="F125" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="19" t="s">
+        <v>392</v>
+      </c>
+      <c r="F125" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A126" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B126" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="C126" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D126" s="19"/>
-      <c r="E126" s="19"/>
-      <c r="F126" s="20" t="s">
+      <c r="B126" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="F126" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="G126" s="19"/>
     </row>
     <row r="127" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>289</v>
+        <v>391</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="F127" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+        <v>394</v>
+      </c>
+      <c r="F127" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>422</v>
+        <v>100</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="F128" s="14" t="s">
-        <v>353</v>
+        <v>107</v>
+      </c>
+      <c r="F128" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G128" s="2" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>291</v>
+        <v>446</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>292</v>
-      </c>
-      <c r="F129" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="F129" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>426</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A131" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="B131" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C131" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D131" s="19"/>
+      <c r="E131" s="19"/>
+      <c r="F131" s="20" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A130" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B130" s="2" t="s">
-        <v>293</v>
-      </c>
-      <c r="C130" s="2" t="s">
-        <v>294</v>
-      </c>
-      <c r="F130" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G130" s="2" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="131" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A131" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B131" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C131" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="F131" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G131" s="19"/>
+    </row>
+    <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>134</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>226</v>
+        <v>289</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="F132" s="5" t="s">
-        <v>141</v>
+        <v>290</v>
+      </c>
+      <c r="F132" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
@@ -4543,13 +4625,16 @@
         <v>134</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>135</v>
+        <v>421</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="F133" s="6" t="s">
-        <v>142</v>
+        <v>422</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F133" s="14" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="134" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4557,13 +4642,13 @@
         <v>134</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="F134" s="4" t="s">
-        <v>140</v>
+        <v>292</v>
+      </c>
+      <c r="F134" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -4571,257 +4656,257 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="C135" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="F135" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G135" s="2" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A136" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="C136" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="F136" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B137" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F137" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B138" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C138" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F138" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B139" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="C139" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A140" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="B140" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C135" s="2" t="s">
+      <c r="C140" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="F135" s="14" t="s">
+      <c r="F140" s="14" t="s">
         <v>353</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="B136" s="19" t="s">
-        <v>136</v>
-      </c>
-      <c r="C136" s="19" t="s">
-        <v>137</v>
-      </c>
-      <c r="D136" s="19"/>
-      <c r="E136" s="19"/>
-      <c r="F136" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="G136" s="19"/>
-    </row>
-    <row r="137" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A137" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B137" s="2" t="s">
-        <v>445</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="F137" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G137" s="2" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="138" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A138" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B138" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="F138" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G138" s="2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A139" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B139" s="2" t="s">
-        <v>354</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>355</v>
-      </c>
-      <c r="F139" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G139" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A140" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B140" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="F140" s="7" t="s">
-        <v>245</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="19" t="s">
-        <v>241</v>
+        <v>134</v>
       </c>
       <c r="B141" s="19" t="s">
-        <v>243</v>
+        <v>136</v>
       </c>
       <c r="C141" s="19" t="s">
-        <v>244</v>
+        <v>137</v>
       </c>
       <c r="D141" s="19"/>
       <c r="E141" s="19"/>
-      <c r="F141" s="26" t="s">
+      <c r="F141" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G141" s="19"/>
+    </row>
+    <row r="142" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A142" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>445</v>
+      </c>
+      <c r="F142" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="G141" s="19" t="s">
+      <c r="G142" s="2" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A143" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B143" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="C143" s="2" t="s">
+        <v>467</v>
+      </c>
+      <c r="F143" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G143" s="2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A144" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B144" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F144" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G144" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B145" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C145" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="F145" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G145" s="2" t="s">
         <v>456</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" s="2" t="s">
+    <row r="146" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A146" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="B146" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146" s="19" t="s">
+        <v>244</v>
+      </c>
+      <c r="D146" s="19"/>
+      <c r="E146" s="19"/>
+      <c r="F146" s="26" t="s">
+        <v>245</v>
+      </c>
+      <c r="G146" s="19" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B147" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C142" s="2" t="s">
+      <c r="C147" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F142" s="7" t="s">
+      <c r="F147" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="G142" s="2" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="2" t="s">
+      <c r="G147" s="2" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B148" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="C143" s="2" t="s">
+      <c r="C148" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="F143" s="7" t="s">
+      <c r="F148" s="7" t="s">
         <v>183</v>
       </c>
-      <c r="G143" s="2" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="19" t="s">
+      <c r="G148" s="2" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="B144" s="19" t="s">
+      <c r="B149" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C144" s="19" t="s">
+      <c r="C149" s="19" t="s">
         <v>275</v>
       </c>
-      <c r="D144" s="19"/>
-      <c r="E144" s="19"/>
-      <c r="F144" s="26" t="s">
+      <c r="D149" s="19"/>
+      <c r="E149" s="19"/>
+      <c r="F149" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="G144" s="19" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A145" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B145" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="F145" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A146" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B146" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="F146" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A147" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B147" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="C147" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="F147" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A148" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B148" s="2" t="s">
-        <v>359</v>
-      </c>
-      <c r="C148" s="2" t="s">
-        <v>360</v>
-      </c>
-      <c r="F148" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="B149" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="C149" s="2" t="s">
-        <v>316</v>
-      </c>
-      <c r="F149" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="G149" s="19" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>329</v>
+        <v>113</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="E150" s="2" t="s">
-        <v>521</v>
-      </c>
-      <c r="F150" s="6" t="s">
-        <v>142</v>
+        <v>122</v>
+      </c>
+      <c r="F150" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
@@ -4829,13 +4914,13 @@
         <v>112</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>313</v>
+        <v>114</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="F151" s="4" t="s">
-        <v>140</v>
+        <v>123</v>
+      </c>
+      <c r="F151" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
@@ -4843,52 +4928,55 @@
         <v>112</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>317</v>
+        <v>395</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>318</v>
+        <v>396</v>
       </c>
       <c r="F152" s="4" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>325</v>
+        <v>359</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="F153" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>360</v>
+      </c>
+      <c r="F153" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>333</v>
+        <v>315</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="F154" s="6" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
+        <v>316</v>
+      </c>
+      <c r="F154" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>321</v>
+        <v>329</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>322</v>
+        <v>330</v>
+      </c>
+      <c r="E155" s="2" t="s">
+        <v>520</v>
       </c>
       <c r="F155" s="6" t="s">
         <v>142</v>
@@ -4899,13 +4987,13 @@
         <v>112</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>472</v>
+        <v>313</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>473</v>
-      </c>
-      <c r="F156" s="6" t="s">
-        <v>142</v>
+        <v>314</v>
+      </c>
+      <c r="F156" s="4" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
@@ -4913,44 +5001,41 @@
         <v>112</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="F157" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A158" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B158" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="C158" s="13" t="s">
-        <v>399</v>
-      </c>
-      <c r="F158" s="7" t="s">
-        <v>400</v>
-      </c>
-      <c r="G158" s="2" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B158" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="F158" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>337</v>
-      </c>
-      <c r="F159" s="5" t="s">
-        <v>141</v>
+        <v>334</v>
+      </c>
+      <c r="F159" s="6" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
@@ -4958,13 +5043,13 @@
         <v>112</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>470</v>
+        <v>321</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>471</v>
-      </c>
-      <c r="F160" s="5" t="s">
-        <v>141</v>
+        <v>322</v>
+      </c>
+      <c r="F160" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
@@ -4972,10 +5057,10 @@
         <v>112</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>115</v>
+        <v>471</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>124</v>
+        <v>472</v>
       </c>
       <c r="F161" s="6" t="s">
         <v>142</v>
@@ -4986,27 +5071,30 @@
         <v>112</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>116</v>
+        <v>342</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="F162" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A163" s="2" t="s">
+        <v>343</v>
+      </c>
+      <c r="F162" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A163" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="B163" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C163" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="F163" s="6" t="s">
-        <v>142</v>
+      <c r="B163" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="C163" s="13" t="s">
+        <v>398</v>
+      </c>
+      <c r="F163" s="7" t="s">
+        <v>399</v>
+      </c>
+      <c r="G163" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
@@ -5014,10 +5102,10 @@
         <v>112</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>118</v>
+        <v>336</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>127</v>
+        <v>337</v>
       </c>
       <c r="F164" s="5" t="s">
         <v>141</v>
@@ -5028,10 +5116,10 @@
         <v>112</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>476</v>
+        <v>470</v>
       </c>
       <c r="F165" s="5" t="s">
         <v>141</v>
@@ -5042,13 +5130,13 @@
         <v>112</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>475</v>
+        <v>115</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>477</v>
-      </c>
-      <c r="F166" s="5" t="s">
-        <v>141</v>
+        <v>124</v>
+      </c>
+      <c r="F166" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
@@ -5056,64 +5144,55 @@
         <v>112</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F167" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="168" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F167" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>408</v>
+        <v>117</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="F168" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G168" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="169" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="F168" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>410</v>
+        <v>118</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="F169" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G169" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="170" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="F169" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>340</v>
+        <v>473</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>341</v>
-      </c>
-      <c r="F170" s="18" t="s">
-        <v>421</v>
-      </c>
-      <c r="G170" s="2" t="s">
-        <v>460</v>
+        <v>475</v>
+      </c>
+      <c r="F170" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
@@ -5121,16 +5200,13 @@
         <v>112</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>331</v>
+        <v>474</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>332</v>
-      </c>
-      <c r="E171" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="F171" s="6" t="s">
-        <v>142</v>
+        <v>476</v>
+      </c>
+      <c r="F171" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
@@ -5138,58 +5214,64 @@
         <v>112</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>323</v>
+        <v>119</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="E172" s="2" t="s">
-        <v>321</v>
-      </c>
-      <c r="F172" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="F172" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A173" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>478</v>
+        <v>407</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="F173" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="F173" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G173" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A174" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>120</v>
+        <v>409</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F174" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>410</v>
+      </c>
+      <c r="F174" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G174" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A175" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>121</v>
+        <v>340</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F175" s="5" t="s">
-        <v>141</v>
+        <v>341</v>
+      </c>
+      <c r="F175" s="18" t="s">
+        <v>420</v>
+      </c>
+      <c r="G175" s="2" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
@@ -5197,16 +5279,16 @@
         <v>112</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="E176" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="F176" s="5" t="s">
-        <v>141</v>
+        <v>319</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
@@ -5214,13 +5296,16 @@
         <v>112</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>348</v>
+        <v>323</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F177" s="16" t="s">
-        <v>361</v>
+        <v>324</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="F177" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
@@ -5228,41 +5313,41 @@
         <v>112</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>414</v>
+        <v>477</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="F178" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>478</v>
+      </c>
+      <c r="F178" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>344</v>
+        <v>120</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="F179" s="5" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+      <c r="F179" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A180" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>327</v>
+        <v>121</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="F180" s="6" t="s">
-        <v>142</v>
+        <v>130</v>
+      </c>
+      <c r="F180" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
@@ -5270,13 +5355,16 @@
         <v>112</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>319</v>
+        <v>338</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="F181" s="14" t="s">
-        <v>353</v>
+        <v>339</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="F181" s="5" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
@@ -5284,61 +5372,52 @@
         <v>112</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>311</v>
+        <v>348</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="F182" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="F182" s="16" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
         <v>112</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>517</v>
+        <v>413</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="F183" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="G183" s="2" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="184" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="F183" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B184" s="19" t="s">
-        <v>424</v>
-      </c>
-      <c r="C184" s="19" t="s">
-        <v>425</v>
-      </c>
-      <c r="D184" s="19"/>
-      <c r="E184" s="19"/>
-      <c r="F184" s="23" t="s">
+      <c r="B184" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C184" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="F184" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G184" s="19"/>
-    </row>
-    <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>132</v>
+        <v>327</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>435</v>
+        <v>328</v>
       </c>
       <c r="F185" s="6" t="s">
         <v>142</v>
@@ -5346,67 +5425,149 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="F186" s="6" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>320</v>
+      </c>
+      <c r="F186" s="14" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>350</v>
+        <v>311</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>351</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>352</v>
+        <v>312</v>
       </c>
       <c r="F187" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>486</v>
+        <v>516</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>487</v>
-      </c>
-      <c r="F188" s="5" t="s">
-        <v>141</v>
+        <v>517</v>
+      </c>
+      <c r="F188" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="G188" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A189" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="B189" s="19" t="s">
+        <v>423</v>
+      </c>
+      <c r="C189" s="19" t="s">
+        <v>424</v>
+      </c>
+      <c r="D189" s="19"/>
+      <c r="E189" s="19"/>
+      <c r="F189" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G189" s="19"/>
+    </row>
+    <row r="190" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B189" s="19" t="s">
+      <c r="B190" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D190" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="F190" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="C191" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D191" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="F191" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="C192" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="D192" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="F192" s="6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>485</v>
+      </c>
+      <c r="C193" s="2" t="s">
+        <v>486</v>
+      </c>
+      <c r="F193" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A194" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="B194" s="19" t="s">
+        <v>405</v>
+      </c>
+      <c r="C194" s="19" t="s">
         <v>406</v>
       </c>
-      <c r="C189" s="19" t="s">
-        <v>407</v>
-      </c>
-      <c r="D189" s="19" t="s">
-        <v>426</v>
-      </c>
-      <c r="E189" s="19"/>
-      <c r="F189" s="20" t="s">
+      <c r="D194" s="19" t="s">
+        <v>425</v>
+      </c>
+      <c r="E194" s="19"/>
+      <c r="F194" s="20" t="s">
         <v>142</v>
       </c>
-      <c r="G189" s="19"/>
+      <c r="G194" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5416,7 +5577,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -5455,105 +5616,121 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>235</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>236</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>235</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>561</v>
       </c>
       <c r="B6" t="s">
-        <v>148</v>
+        <v>562</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s">
-        <v>308</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>384</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
-        <v>385</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>383</v>
       </c>
       <c r="B9" t="s">
-        <v>149</v>
+        <v>384</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>497</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>498</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>94</v>
+        <v>556</v>
       </c>
       <c r="B11" t="s">
-        <v>200</v>
+        <v>557</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>134</v>
+        <v>496</v>
       </c>
       <c r="B12" t="s">
-        <v>150</v>
+        <v>497</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>241</v>
+        <v>94</v>
       </c>
       <c r="B13" t="s">
-        <v>242</v>
+        <v>200</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>109</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>112</v>
+        <v>241</v>
       </c>
       <c r="B15" t="s">
-        <v>199</v>
+        <v>242</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>109</v>
+      </c>
+      <c r="B16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>131</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>